<commit_message>
'Stability' -> 'Scalability' in Documentation/Sensors' precision.xlsx.
</commit_message>
<xml_diff>
--- a/Documentation/Sensors' precision.xlsx
+++ b/Documentation/Sensors' precision.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bureau\educat_irsensor\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDAF752-4DB5-4BA6-98E6-7FA8C637C939}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD21FCF-A547-4602-B7F4-42C7DDE735F7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,9 +61,6 @@
     <t>max</t>
   </si>
   <si>
-    <t>std deviation / distance_real</t>
-  </si>
-  <si>
     <t>mean</t>
   </si>
   <si>
@@ -92,6 +89,9 @@
   </si>
   <si>
     <t>Plastique Gris</t>
+  </si>
+  <si>
+    <t>scalability</t>
   </si>
 </sst>
 </file>
@@ -2411,7 +2411,7 @@
                 <a:uFillTx/>
                 <a:latin typeface="Calibri"/>
               </a:rPr>
-              <a:t>Stability from Sensor 4</a:t>
+              <a:t>Scalability from Sensor 4</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2448,7 +2448,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>std deviation / distance_real</c:v>
+                  <c:v>scalability</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6392,7 +6392,7 @@
                 <a:uFillTx/>
                 <a:latin typeface="Calibri"/>
               </a:rPr>
-              <a:t>Stability from Sensor 1</a:t>
+              <a:t>Scalability from Sensor 1</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -6429,7 +6429,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>std deviation / distance_real</c:v>
+                  <c:v>scalability</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -8669,7 +8669,7 @@
                 <a:uFillTx/>
                 <a:latin typeface="Calibri"/>
               </a:rPr>
-              <a:t>Stability from Sensor 2</a:t>
+              <a:t>Scalability from Sensor 2</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -8706,7 +8706,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>std deviation / distance_real</c:v>
+                  <c:v>scalability</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -11519,7 +11519,7 @@
                 <a:uFillTx/>
                 <a:latin typeface="Calibri"/>
               </a:rPr>
-              <a:t>Stability from Sensor 3</a:t>
+              <a:t>Scalability from Sensor 3</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -11556,7 +11556,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>std deviation / distance_real</c:v>
+                  <c:v>scalability</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -12092,7 +12092,7 @@
                 <a:uFillTx/>
                 <a:latin typeface="Calibri"/>
               </a:rPr>
-              <a:t>Stability from Sensor 4</a:t>
+              <a:t>Scalability from Sensor 4</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -12129,7 +12129,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>std deviation / distance_real</c:v>
+                  <c:v>scalability</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -16045,7 +16045,7 @@
                 <a:uFillTx/>
                 <a:latin typeface="Calibri"/>
               </a:rPr>
-              <a:t>Stability from Sensor 1</a:t>
+              <a:t>Scalability from Sensor 1</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -18470,7 +18470,7 @@
                 <a:uFillTx/>
                 <a:latin typeface="Calibri"/>
               </a:rPr>
-              <a:t>Stability from Sensor 1</a:t>
+              <a:t>Scalability from Sensor 1</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -18507,7 +18507,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>std deviation / distance_real</c:v>
+                  <c:v>scalability</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -19043,7 +19043,7 @@
                 <a:uFillTx/>
                 <a:latin typeface="Calibri"/>
               </a:rPr>
-              <a:t>Stability from Sensor 2</a:t>
+              <a:t>Scalability from Sensor 2</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -21466,7 +21466,7 @@
                 <a:uFillTx/>
                 <a:latin typeface="Calibri"/>
               </a:rPr>
-              <a:t>Stability from Sensor 3</a:t>
+              <a:t>Scalability from Sensor 3</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -22213,7 +22213,7 @@
                 <a:uFillTx/>
                 <a:latin typeface="Calibri"/>
               </a:rPr>
-              <a:t>Stability from Sensor 4</a:t>
+              <a:t>Scalability from Sensor 4</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -27028,7 +27028,7 @@
                 <a:uFillTx/>
                 <a:latin typeface="Calibri"/>
               </a:rPr>
-              <a:t>Stability without protection</a:t>
+              <a:t>Scalability without protection</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -31654,7 +31654,7 @@
                 <a:uFillTx/>
                 <a:latin typeface="Calibri"/>
               </a:rPr>
-              <a:t>Stability with protection</a:t>
+              <a:t>Scalability with protection</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -32803,6 +32803,33 @@
             <c:symbol val="circle"/>
             <c:size val="5"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>comparision_different_materials!$D$4:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>53.44</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>103.44</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>153.44</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>203.44</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>253.44</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>303.44</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>comparision_different_materials!$D$4:$D$9</c:f>
@@ -32864,6 +32891,33 @@
             <c:symbol val="circle"/>
             <c:size val="5"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>comparision_different_materials!$D$4:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>53.44</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>103.44</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>153.44</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>203.44</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>253.44</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>303.44</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>comparision_different_materials!$M$4:$M$9</c:f>
@@ -32925,6 +32979,33 @@
             <c:symbol val="circle"/>
             <c:size val="5"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>comparision_different_materials!$D$4:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>53.44</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>103.44</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>153.44</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>203.44</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>253.44</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>303.44</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>comparision_different_materials!$M$10:$M$15</c:f>
@@ -32986,6 +33067,33 @@
             <c:symbol val="circle"/>
             <c:size val="5"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>comparision_different_materials!$D$4:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>53.44</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>103.44</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>153.44</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>203.44</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>253.44</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>303.44</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>comparision_different_materials!$M$16:$M$21</c:f>
@@ -33047,6 +33155,33 @@
             <c:symbol val="circle"/>
             <c:size val="5"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>comparision_different_materials!$D$4:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>53.44</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>103.44</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>153.44</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>203.44</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>253.44</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>303.44</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>comparision_different_materials!$M$22:$M$27</c:f>
@@ -33108,6 +33243,33 @@
             <c:symbol val="circle"/>
             <c:size val="5"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>comparision_different_materials!$D$4:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>53.44</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>103.44</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>153.44</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>203.44</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>253.44</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>303.44</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>comparision_different_materials!$M$28:$M$33</c:f>
@@ -33309,6 +33471,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -34057,7 +34220,7 @@
                 <a:uFillTx/>
                 <a:latin typeface="Calibri"/>
               </a:rPr>
-              <a:t>Stability from Sensor 2</a:t>
+              <a:t>Scalability from Sensor 2</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -34094,7 +34257,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>std deviation / distance_real</c:v>
+                  <c:v>scalability</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -36334,7 +36497,7 @@
                 <a:uFillTx/>
                 <a:latin typeface="Calibri"/>
               </a:rPr>
-              <a:t>Stability from Sensor 3</a:t>
+              <a:t>Scalability from Sensor 3</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -36371,7 +36534,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>std deviation / distance_real</c:v>
+                  <c:v>scalability</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -38525,8 +38688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AU95"/>
   <sheetViews>
-    <sheetView topLeftCell="L4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AV79" sqref="AV79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -38736,13 +38899,13 @@
         <v>8</v>
       </c>
       <c r="K4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="M4" s="8" t="s">
         <v>10</v>
-      </c>
-      <c r="M4" s="8" t="s">
-        <v>11</v>
       </c>
       <c r="N4" s="7">
         <f>$D4</f>
@@ -38774,7 +38937,7 @@
       </c>
       <c r="U4" s="7" t="str">
         <f>$K4</f>
-        <v>std deviation / distance_real</v>
+        <v>scalability</v>
       </c>
       <c r="V4" s="7" t="str">
         <f>$L4</f>
@@ -38822,7 +38985,7 @@
       </c>
       <c r="AG4" s="7" t="str">
         <f>$K4</f>
-        <v>std deviation / distance_real</v>
+        <v>scalability</v>
       </c>
       <c r="AH4" s="7" t="str">
         <f>$L4</f>
@@ -38862,7 +39025,7 @@
       </c>
       <c r="AQ4" s="7" t="str">
         <f>$K4</f>
-        <v>std deviation / distance_real</v>
+        <v>scalability</v>
       </c>
       <c r="AR4" s="7" t="str">
         <f>$L4</f>
@@ -42774,7 +42937,7 @@
     </row>
     <row r="30" spans="2:47" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
       <c r="B30" s="30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C30" s="31">
         <v>3.44</v>
@@ -42900,7 +43063,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:AU95"/>
   <sheetViews>
-    <sheetView topLeftCell="M17" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="B40" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="W144" sqref="W144"/>
     </sheetView>
   </sheetViews>
@@ -43126,7 +43289,7 @@
       </c>
       <c r="K4" s="5" t="str">
         <f>without_protection!$K4</f>
-        <v>std deviation / distance_real</v>
+        <v>scalability</v>
       </c>
       <c r="L4" s="5" t="str">
         <f>without_protection!$L4</f>
@@ -43166,7 +43329,7 @@
       </c>
       <c r="U4" s="5" t="str">
         <f>without_protection!$K4</f>
-        <v>std deviation / distance_real</v>
+        <v>scalability</v>
       </c>
       <c r="V4" s="5" t="str">
         <f>without_protection!$L4</f>
@@ -43214,7 +43377,7 @@
       </c>
       <c r="AG4" s="5" t="str">
         <f>without_protection!$K4</f>
-        <v>std deviation / distance_real</v>
+        <v>scalability</v>
       </c>
       <c r="AH4" s="5" t="str">
         <f>without_protection!$L4</f>
@@ -43254,7 +43417,7 @@
       </c>
       <c r="AQ4" s="5" t="str">
         <f>without_protection!$K4</f>
-        <v>std deviation / distance_real</v>
+        <v>scalability</v>
       </c>
       <c r="AR4" s="5" t="str">
         <f>without_protection!$L4</f>
@@ -47328,7 +47491,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>
@@ -47347,7 +47510,7 @@
   <dimension ref="B1:N38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -47360,7 +47523,7 @@
     <row r="1" spans="2:14" ht="15" thickBot="1"/>
     <row r="2" spans="2:14" ht="16.5" thickTop="1" thickBot="1">
       <c r="B2" s="84" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="85" t="str">
         <f>without_protection!$B3</f>
@@ -47368,7 +47531,7 @@
       </c>
       <c r="D2" s="85"/>
       <c r="E2" s="86" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" s="86"/>
       <c r="G2" s="86"/>
@@ -47420,7 +47583,7 @@
       </c>
       <c r="L3" s="5" t="str">
         <f>without_protection!$K4</f>
-        <v>std deviation / distance_real</v>
+        <v>scalability</v>
       </c>
       <c r="M3" s="5" t="str">
         <f>without_protection!$L4</f>
@@ -47433,7 +47596,7 @@
     </row>
     <row r="4" spans="2:14" ht="16.5" thickTop="1" thickBot="1">
       <c r="B4" s="87" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="35">
         <f>50</f>
@@ -47709,7 +47872,7 @@
     </row>
     <row r="10" spans="2:14" ht="15.75" thickBot="1">
       <c r="B10" s="88" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="46">
         <f t="shared" ref="C10:D15" si="6">C4</f>
@@ -47987,7 +48150,7 @@
     </row>
     <row r="16" spans="2:14" ht="15.75" thickBot="1">
       <c r="B16" s="83" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" s="35">
         <f t="shared" ref="C16:D21" si="7">C4</f>
@@ -48265,7 +48428,7 @@
     </row>
     <row r="22" spans="2:14" ht="15.75" thickBot="1">
       <c r="B22" s="83" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C22" s="35">
         <f t="shared" ref="C22:C27" si="8">C16</f>
@@ -48543,7 +48706,7 @@
     </row>
     <row r="28" spans="2:14" ht="15.75" thickBot="1">
       <c r="B28" s="83" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C28" s="64">
         <f t="shared" ref="C28:D33" si="10">C4</f>

</xml_diff>